<commit_message>
run without internal server errors, only inaccuracies in data present
</commit_message>
<xml_diff>
--- a/data/sql.xlsx
+++ b/data/sql.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -482,6 +482,48 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>SELECT "id", "customer_number", "customer_name", "client_id", "client_name", "captain_name", "delivery_date", "order_status", "shop_to_delivery_km", "order_created_at", "order_accepted_at", "start_ride_at", "reached_shop_at", "order_picked_at", "shipped_at", "reached_dest_at", "final_status_at", "cancellation_reason" FROM "updated_table" WHERE "client_name" = 'MC DONALDS' AND "order_created_at" &gt;= (CURRENT_TIMESTAMP - INTERVAL '1 year') ORDER BY "order_created_at" DESC LIMIT 10;</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>SELECT MAX("order_created_at") AS "Last_Order_Time" FROM "updated_table" WHERE "client_name" = 'MC DONALDS';</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>SELECT "delivery_date" FROM "updated_table" WHERE "client_name" = 'MC DONALDS' AND "delivery_date" = (SELECT MAX("delivery_date") FROM "updated_table" WHERE "client_name" = 'MC DONALDS');</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>SELECT "id", "customer_number", "customer_name", "client_id", "client_name", "captain_name", "delivery_date", "order_status", "shop_to_delivery_km", "order_created_at", "order_accepted_at", "start_ride_at", "reached_shop_at", "order_picked_at", "shipped_at", "reached_dest_at", "final_status_at", "cancellation_reason" FROM "updated_table" WHERE "client_name" = 'MC DONALDS' AND "order_created_at" &lt;= '2025-09-12 12:37:40.233648' ORDER BY "order_created_at" DESC LIMIT 10;</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>SELECT "id", "customer_number", "customer_name", "client_id", "client_name", "captain_name", "delivery_date", "order_status", "shop_to_delivery_km", "order_created_at", "order_accepted_at", "start_ride_at", "reached_shop_at", "order_picked_at", "shipped_at", "reached_dest_at", "final_status_at", "cancellation_reason" FROM "updated_table" WHERE "client_name" = 'MC DONALDS' AND "order_created_at" &lt;= '2025-09-12 12:39:10.848770' ORDER BY "order_created_at" DESC LIMIT 10;</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>SELECT "order_created_at" FROM "updated_table" WHERE "client_name" = 'MC DONALDS' AND "order_created_at" = (SELECT MAX("order_created_at") FROM "updated_table" WHERE "client_name" = 'MC DONALDS');</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
push to test branch
</commit_message>
<xml_diff>
--- a/data/sql.xlsx
+++ b/data/sql.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A131"/>
+  <dimension ref="A1:A136"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1482,6 +1482,43 @@
         </is>
       </c>
     </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>```sql
+SELECT "order_status" FROM "updated_table" WHERE "client_name" = 'MC DONALDS' AND "order_created_at" &gt;= '2025-07-01' AND "order_created_at" &lt; '2025-08-01' LIMIT 1;
+```</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>SELECT "order_status" FROM "updated_table" WHERE "client_name" = 'MC DONALDS' AND "final_status_at" &gt;= '2025-07-01 00:00:00' AND "final_status_at" &lt; '2025-08-01 00:00:00' ORDER BY "final_status_at" DESC LIMIT 1;</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>SELECT "id" AS order_number FROM "updated_table" WHERE "client_name" = 'MC DONALDS' AND EXTRACT(MONTH FROM "order_created_at") = 7 ORDER BY "order_created_at" DESC LIMIT 1;</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>SELECT "order_status" FROM "updated_table" WHERE "client_name" = 'MC DONALDS' AND "id" = 1823383 LIMIT 1;</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>SELECT "id", "order_status", "delivery_date", "order_created_at", "order_accepted_at", "start_ride_at", "reached_shop_at", "order_picked_at", "shipped_at", "reached_dest_at", "final_status_at", "customer_number", "customer_name", "client_id", "captain_name", "shop_to_delivery_km", "cancellation_reason" FROM "updated_table" WHERE "client_name" = 'MC DONALDS' AND "order_created_at" &gt;= '2025-07-01' AND "order_created_at" &lt; '2025-08-01' LIMIT 1;</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>